<commit_message>
Upgrade simple 2 example
</commit_message>
<xml_diff>
--- a/source_data/simple_2.xlsx
+++ b/source_data/simple_2.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8C4B45-CD7B-3E49-A59A-C3FBFC857B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDE78A7-D850-144D-9929-4569F5DFC57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16580" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="7380" yWindow="680" windowWidth="28800" windowHeight="16580" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="study" sheetId="2" r:id="rId1"/>
+    <sheet name="studyIdentifiers" sheetId="3" r:id="rId2"/>
+    <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
+    <sheet name="soa" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -101,18 +104,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>BC:PE 1</t>
-  </si>
-  <si>
-    <t>BC:PE 2</t>
-  </si>
-  <si>
-    <t>BC:Weight</t>
-  </si>
-  <si>
-    <t>BC:Height</t>
-  </si>
-  <si>
     <t>BC/Profile</t>
   </si>
   <si>
@@ -123,13 +114,118 @@
   </si>
   <si>
     <t>1 .. N</t>
+  </si>
+  <si>
+    <t>BC: PE 1, BC: PE 2, BC: Weight, BC: Height</t>
+  </si>
+  <si>
+    <t>studyTitle</t>
+  </si>
+  <si>
+    <t>studyVersion</t>
+  </si>
+  <si>
+    <t>studyType</t>
+  </si>
+  <si>
+    <t>studyPhase</t>
+  </si>
+  <si>
+    <t>Simple Test 1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>C98388=Interventional Study</t>
+  </si>
+  <si>
+    <t>C15602=Phase III Trial</t>
+  </si>
+  <si>
+    <t>organisationIdentifierScheme</t>
+  </si>
+  <si>
+    <t>organisationIdentifier</t>
+  </si>
+  <si>
+    <t>organisationName</t>
+  </si>
+  <si>
+    <t>organisationType</t>
+  </si>
+  <si>
+    <t>studyIdentifier</t>
+  </si>
+  <si>
+    <t>USGOV</t>
+  </si>
+  <si>
+    <t>CT-GOV</t>
+  </si>
+  <si>
+    <t>ClinicalTrials.gov</t>
+  </si>
+  <si>
+    <t>Registry</t>
+  </si>
+  <si>
+    <t>NCT12345678</t>
+  </si>
+  <si>
+    <t>therapeuticAreas</t>
+  </si>
+  <si>
+    <t>Not supported yet</t>
+  </si>
+  <si>
+    <t>studyDesignRationale</t>
+  </si>
+  <si>
+    <t>"Study design rationale put here"</t>
+  </si>
+  <si>
+    <t>studyDesignBlindingScheme</t>
+  </si>
+  <si>
+    <t>C49659=OPEN LABEL</t>
+  </si>
+  <si>
+    <t>trialIntentTypes</t>
+  </si>
+  <si>
+    <t>C15714=BASIC SCIENCE, C139174=DEVICE FEASIBILITY</t>
+  </si>
+  <si>
+    <t>trialTypes</t>
+  </si>
+  <si>
+    <t>C12345=Observational</t>
+  </si>
+  <si>
+    <t>interventionModel</t>
+  </si>
+  <si>
+    <t>C12346=None</t>
+  </si>
+  <si>
+    <t>Follow-Up</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>cell</t>
+  </si>
+  <si>
+    <t>Placebo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -139,6 +235,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -172,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -190,6 +294,26 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -514,14 +638,257 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED78087-5EC8-E249-9405-08BCDA276930}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="4" width="30.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370D0E30-FAA2-1D42-9C6C-E637CF86137F}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A66060-C34D-B74B-9573-D0BFE7F2808B}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="5" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,80 +900,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="15"/>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="7"/>
+      <c r="D2" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="15"/>
       <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="9"/>
+      <c r="D5" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="17"/>
       <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
@@ -621,8 +988,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -633,12 +1000,12 @@
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
@@ -660,18 +1027,18 @@
         <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
+      <c r="C10" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
@@ -681,66 +1048,6 @@
       </c>
       <c r="F10" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update simple 2 example
</commit_message>
<xml_diff>
--- a/source_data/simple_2.xlsx
+++ b/source_data/simple_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5C1333-2A9B-A447-B105-6F566030A44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6606F3-9A58-E14F-B27B-2073FCD62D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43700" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="43700" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="studyDesignOE" sheetId="7" r:id="rId7"/>
     <sheet name="studyDesignEstimands" sheetId="8" r:id="rId8"/>
     <sheet name="studyDesignProcedures" sheetId="10" r:id="rId9"/>
-    <sheet name="configuration" sheetId="9" r:id="rId10"/>
+    <sheet name="studyDesignEncounters" sheetId="11" r:id="rId10"/>
+    <sheet name="configuration" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="173">
   <si>
     <t>Epoch</t>
   </si>
@@ -59,9 +60,6 @@
     <t>Cycle End Rule</t>
   </si>
   <si>
-    <t>Visit Label</t>
-  </si>
-  <si>
     <t>Day 1</t>
   </si>
   <si>
@@ -71,9 +69,6 @@
     <t>P: +14 Days</t>
   </si>
   <si>
-    <t>Visit Window</t>
-  </si>
-  <si>
     <t>-2..2 Days</t>
   </si>
   <si>
@@ -107,9 +102,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>BC/Profile</t>
-  </si>
-  <si>
     <t>Disease Progression</t>
   </si>
   <si>
@@ -516,6 +508,63 @@
   </si>
   <si>
     <t>Simple Cycle Test</t>
+  </si>
+  <si>
+    <t>encounterName</t>
+  </si>
+  <si>
+    <t>encounterDescription</t>
+  </si>
+  <si>
+    <t>encounterType</t>
+  </si>
+  <si>
+    <t>encounterEnvironmentalSetting</t>
+  </si>
+  <si>
+    <t>encounterContactModes</t>
+  </si>
+  <si>
+    <t>transitionStartRule</t>
+  </si>
+  <si>
+    <t>transitionEndRule</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>Visit</t>
+  </si>
+  <si>
+    <t>CLINIC</t>
+  </si>
+  <si>
+    <t>In Person</t>
+  </si>
+  <si>
+    <t>IEs passed</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>Follow up</t>
+  </si>
+  <si>
+    <t>Subject identified</t>
+  </si>
+  <si>
+    <t>BC/Procedure/Timeline</t>
+  </si>
+  <si>
+    <t>Encounter xref</t>
+  </si>
+  <si>
+    <t>Window</t>
   </si>
 </sst>
 </file>
@@ -588,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -597,9 +646,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -645,18 +691,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -677,6 +714,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1006,132 +1050,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
         <v>107</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="B9" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C9" s="18" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="E9" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="F9" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="G9" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="H9" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="F9" s="20" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="B10" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="C10" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>122</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="21">
+      <c r="G10" s="20">
         <v>40179</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="16" t="s">
+      <c r="A11" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>121</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>124</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G11" s="21">
+        <v>122</v>
+      </c>
+      <c r="G11" s="20">
         <v>40544</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1140,6 +1184,121 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF4C881-F99F-AB40-940B-2531415A94FC}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="16" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="3" customWidth="1"/>
+    <col min="6" max="8" width="27.33203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6879B0C-C67A-EA45-AA03-0AE5CE49C17A}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1153,19 +1312,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>131</v>
+      <c r="A1" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>131</v>
+      <c r="A2" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1191,40 +1350,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>49</v>
+      <c r="F1" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1236,7 +1395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A66060-C34D-B74B-9573-D0BFE7F2808B}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -1247,138 +1406,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="B4" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="B5" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B6" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="B12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1402,177 +1561,177 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" style="3" customWidth="1"/>
     <col min="4" max="8" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="27"/>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="5" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="5" t="s">
+      <c r="F8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="C10" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1603,73 +1762,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>54</v>
+      <c r="A1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>61</v>
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
         <v>59</v>
-      </c>
-      <c r="D5" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1695,71 +1854,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>76</v>
+        <v>66</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1781,46 +1940,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="D2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1847,55 +2006,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
         <v>94</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>95</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>96</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>97</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>98</v>
-      </c>
-      <c r="F2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1916,58 +2075,58 @@
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24" style="10" customWidth="1"/>
+    <col min="4" max="4" width="24" style="9" customWidth="1"/>
     <col min="5" max="5" width="29.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="26" t="s">
+      <c r="A1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>151</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="E3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="6"/>
+      <c r="B5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>